<commit_message>
Included data base functionality..
</commit_message>
<xml_diff>
--- a/data/Market Symbols.xlsx
+++ b/data/Market Symbols.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanumaprasad\Desktop\Ui Path Practice\Yahoo Finance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanumaprasad\Desktop\Ui Path Practice\Yahoo Finance\MarketData\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E41765-0655-4004-9498-F6336D55555B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A51460-9074-4851-B616-67C580454E14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="1185" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4350" yWindow="1200" windowWidth="15375" windowHeight="9720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Symbols" sheetId="1" r:id="rId1"/>
@@ -357,7 +357,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>